<commit_message>
commit - Final commit from pc gefco
</commit_message>
<xml_diff>
--- a/___VALEO/doc/MEMOIRE_Synthèse-methodes.xlsx
+++ b/___VALEO/doc/MEMOIRE_Synthèse-methodes.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EXED\Training\___VALEO\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4131A9BC-0D1F-437D-BC31-C6C877E9EF54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6540A16C-321A-488A-AD28-620937B742DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="4920" xr2:uid="{16BD2419-3F19-4547-8D09-223C8CB1DE92}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="4920" firstSheet="1" activeTab="1" xr2:uid="{16BD2419-3F19-4547-8D09-223C8CB1DE92}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="All" sheetId="1" r:id="rId1"/>
+    <sheet name="Performance" sheetId="3" r:id="rId2"/>
+    <sheet name="Autre mesures" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="431">
   <si>
     <t>roc_auc</t>
   </si>
@@ -748,13 +750,611 @@
   </si>
   <si>
     <t>0.645</t>
+  </si>
+  <si>
+    <t>Discriminatif</t>
+  </si>
+  <si>
+    <t>Generatif</t>
+  </si>
+  <si>
+    <t>Paramétrique 
+Oui / Non</t>
+  </si>
+  <si>
+    <t>Bagging / Boosting</t>
+  </si>
+  <si>
+    <t>SmoteBLine / R. undersampling</t>
+  </si>
+  <si>
+    <t>Lazy 
+Eager</t>
+  </si>
+  <si>
+    <t>SmoteEnn / SmoteTomek</t>
+  </si>
+  <si>
+    <t>bagging + 
+under sampling natif à l'algorithme</t>
+  </si>
+  <si>
+    <t>bagging + boosting + 
+under sampling natif à l'algorithme</t>
+  </si>
+  <si>
+    <t>boosting + 
+under sampling natif à l'algorithme</t>
+  </si>
+  <si>
+    <t>bagging + SmoteTomek</t>
+  </si>
+  <si>
+    <t>bagging + SmoteEnn</t>
+  </si>
+  <si>
+    <t>bagging + SmoteBLine + 
+Random undersampling</t>
+  </si>
+  <si>
+    <t>SmoteEnn</t>
+  </si>
+  <si>
+    <t>RF + BLineSmote +
+RandUnderSampler</t>
+  </si>
+  <si>
+    <t>Reg Logistique + 
+SmoteENN</t>
+  </si>
+  <si>
+    <t>GaussianNB + 
+SmoteENN</t>
+  </si>
+  <si>
+    <t>Reg Logistique +
+ SmoteENN</t>
+  </si>
+  <si>
+    <t>SVM(rbf) + 
+SmoteENN</t>
+  </si>
+  <si>
+    <t>itre</t>
+  </si>
+  <si>
+    <t>Oui pour RL
+Non (SmtENN)</t>
+  </si>
+  <si>
+    <t>Oui pour GNB
+Non (SmtENN)</t>
+  </si>
+  <si>
+    <t>0.0429</t>
+  </si>
+  <si>
+    <t>0.7569</t>
+  </si>
+  <si>
+    <t>0.0206</t>
+  </si>
+  <si>
+    <t>0.0202</t>
+  </si>
+  <si>
+    <t>0.2787</t>
+  </si>
+  <si>
+    <t>0.0188</t>
+  </si>
+  <si>
+    <t>0.0337</t>
+  </si>
+  <si>
+    <t>0.5742</t>
+  </si>
+  <si>
+    <t>0.0187</t>
+  </si>
+  <si>
+    <t>0.0351</t>
+  </si>
+  <si>
+    <t>0.0199</t>
+  </si>
+  <si>
+    <t>0.9905</t>
+  </si>
+  <si>
+    <t>0.0441</t>
+  </si>
+  <si>
+    <t>0.0844</t>
+  </si>
+  <si>
+    <t>0.9539</t>
+  </si>
+  <si>
+    <t>0.6999</t>
+  </si>
+  <si>
+    <t>0.4981</t>
+  </si>
+  <si>
+    <t>0.224</t>
+  </si>
+  <si>
+    <t>0.6725</t>
+  </si>
+  <si>
+    <t>0.5400</t>
+  </si>
+  <si>
+    <t>0.0382</t>
+  </si>
+  <si>
+    <t>0.8451</t>
+  </si>
+  <si>
+    <t>0.8107</t>
+  </si>
+  <si>
+    <t>0.0267</t>
+  </si>
+  <si>
+    <t>0.0518</t>
+  </si>
+  <si>
+    <t>0.8423</t>
+  </si>
+  <si>
+    <t>0.7027</t>
+  </si>
+  <si>
+    <t>0.6116</t>
+  </si>
+  <si>
+    <t>0.0390</t>
+  </si>
+  <si>
+    <t>0.7491</t>
+  </si>
+  <si>
+    <t>0.6701</t>
+  </si>
+  <si>
+    <t>0.6200</t>
+  </si>
+  <si>
+    <t>0.0159</t>
+  </si>
+  <si>
+    <t>0.0310</t>
+  </si>
+  <si>
+    <t>4.1627</t>
+  </si>
+  <si>
+    <t>0.3700</t>
+  </si>
+  <si>
+    <t>21.0091</t>
+  </si>
+  <si>
+    <t>3.7217</t>
+  </si>
+  <si>
+    <t>0.7535</t>
+  </si>
+  <si>
+    <t>0.0270</t>
+  </si>
+  <si>
+    <t>0.0522</t>
+  </si>
+  <si>
+    <t>0.8075</t>
+  </si>
+  <si>
+    <t>0.6694</t>
+  </si>
+  <si>
+    <t>0.5295</t>
+  </si>
+  <si>
+    <t>0.0363</t>
+  </si>
+  <si>
+    <t>0.7178</t>
+  </si>
+  <si>
+    <t>0.6483</t>
+  </si>
+  <si>
+    <t>0.5600</t>
+  </si>
+  <si>
+    <t>0.0153</t>
+  </si>
+  <si>
+    <t>0.0297</t>
+  </si>
+  <si>
+    <t>21.6472</t>
+  </si>
+  <si>
+    <t>8.7849</t>
+  </si>
+  <si>
+    <t>0.8164</t>
+  </si>
+  <si>
+    <t>0.6560</t>
+  </si>
+  <si>
+    <t>0.0276</t>
+  </si>
+  <si>
+    <t>0.0530</t>
+  </si>
+  <si>
+    <t>0.8245</t>
+  </si>
+  <si>
+    <t>0.6761</t>
+  </si>
+  <si>
+    <t>0.4942</t>
+  </si>
+  <si>
+    <t>0.7421</t>
+  </si>
+  <si>
+    <t>0.6727</t>
+  </si>
+  <si>
+    <t>0.0362</t>
+  </si>
+  <si>
+    <t>22.5675</t>
+  </si>
+  <si>
+    <t>6.0610</t>
+  </si>
+  <si>
+    <t>0.8348</t>
+  </si>
+  <si>
+    <t>0.9120</t>
+  </si>
+  <si>
+    <t>0.0426</t>
+  </si>
+  <si>
+    <t>0.8264</t>
+  </si>
+  <si>
+    <t>0.6478</t>
+  </si>
+  <si>
+    <t>0.6237</t>
+  </si>
+  <si>
+    <t>0.0148</t>
+  </si>
+  <si>
+    <t>0.0290</t>
+  </si>
+  <si>
+    <t>0.7155</t>
+  </si>
+  <si>
+    <t>0.6268</t>
+  </si>
+  <si>
+    <t>0.0117</t>
+  </si>
+  <si>
+    <t>0.0230</t>
+  </si>
+  <si>
+    <t>23.7319</t>
+  </si>
+  <si>
+    <t>4.1073</t>
+  </si>
+  <si>
+    <t>0.8590</t>
+  </si>
+  <si>
+    <t>0.7081</t>
+  </si>
+  <si>
+    <t>0.0356</t>
+  </si>
+  <si>
+    <t>0.0677</t>
+  </si>
+  <si>
+    <t>0.8578</t>
+  </si>
+  <si>
+    <t>0.6798</t>
+  </si>
+  <si>
+    <t>0.4316</t>
+  </si>
+  <si>
+    <t>0.0213</t>
+  </si>
+  <si>
+    <t>0.0406</t>
+  </si>
+  <si>
+    <t>0.7532</t>
+  </si>
+  <si>
+    <t>0.6577</t>
+  </si>
+  <si>
+    <t>0.5000</t>
+  </si>
+  <si>
+    <t>0.0194</t>
+  </si>
+  <si>
+    <t>29.6008</t>
+  </si>
+  <si>
+    <t>0.3572</t>
+  </si>
+  <si>
+    <t>0.8666</t>
+  </si>
+  <si>
+    <t>0.6275</t>
+  </si>
+  <si>
+    <t>0.0410</t>
+  </si>
+  <si>
+    <t>0.0769</t>
+  </si>
+  <si>
+    <t>0.8687</t>
+  </si>
+  <si>
+    <t>0.6843</t>
+  </si>
+  <si>
+    <t>0.0427</t>
+  </si>
+  <si>
+    <t>0.7401</t>
+  </si>
+  <si>
+    <t>0.6189</t>
+  </si>
+  <si>
+    <t>0.3800</t>
+  </si>
+  <si>
+    <t>0.0364</t>
+  </si>
+  <si>
+    <t>23.8095</t>
+  </si>
+  <si>
+    <t>0.3581</t>
+  </si>
+  <si>
+    <t>0.7984</t>
+  </si>
+  <si>
+    <t>0.1585</t>
+  </si>
+  <si>
+    <t>0.1018</t>
+  </si>
+  <si>
+    <t>0.1229</t>
+  </si>
+  <si>
+    <t>0.7835</t>
+  </si>
+  <si>
+    <t>0.6341</t>
+  </si>
+  <si>
+    <t>0.0237</t>
+  </si>
+  <si>
+    <t>0.0210</t>
+  </si>
+  <si>
+    <t>0.6605</t>
+  </si>
+  <si>
+    <t>0.5308</t>
+  </si>
+  <si>
+    <t>0.0800</t>
+  </si>
+  <si>
+    <t>0.0308</t>
+  </si>
+  <si>
+    <t>0.0444</t>
+  </si>
+  <si>
+    <t>3.8254</t>
+  </si>
+  <si>
+    <t>0.3894</t>
+  </si>
+  <si>
+    <t>0.7439</t>
+  </si>
+  <si>
+    <t>0.6644</t>
+  </si>
+  <si>
+    <t>0.7332</t>
+  </si>
+  <si>
+    <t>0.7133</t>
+  </si>
+  <si>
+    <t>0.6352</t>
+  </si>
+  <si>
+    <t>0.7671</t>
+  </si>
+  <si>
+    <t>0.6636</t>
+  </si>
+  <si>
+    <t>0.0143</t>
+  </si>
+  <si>
+    <t>0.0279</t>
+  </si>
+  <si>
+    <t>60.4653</t>
+  </si>
+  <si>
+    <t>0.1571</t>
+  </si>
+  <si>
+    <t>0.9399</t>
+  </si>
+  <si>
+    <t>0.1244</t>
+  </si>
+  <si>
+    <t>0.9373</t>
+  </si>
+  <si>
+    <t>0.6400</t>
+  </si>
+  <si>
+    <t>0.2708</t>
+  </si>
+  <si>
+    <t>0.5854</t>
+  </si>
+  <si>
+    <t>0.9384</t>
+  </si>
+  <si>
+    <t>0.0105</t>
+  </si>
+  <si>
+    <t>0.0208</t>
+  </si>
+  <si>
+    <t>0.6665</t>
+  </si>
+  <si>
+    <t>0.5715</t>
+  </si>
+  <si>
+    <t>0.9335</t>
+  </si>
+  <si>
+    <t>0.0207</t>
+  </si>
+  <si>
+    <t>0.6418</t>
+  </si>
+  <si>
+    <t>0.5664</t>
+  </si>
+  <si>
+    <t>0.9400</t>
+  </si>
+  <si>
+    <t>0.0084</t>
+  </si>
+  <si>
+    <t>0.0167</t>
+  </si>
+  <si>
+    <t>24.2888</t>
+  </si>
+  <si>
+    <t>0.1463</t>
+  </si>
+  <si>
+    <t>0.9648</t>
+  </si>
+  <si>
+    <t>0.9535</t>
+  </si>
+  <si>
+    <t>0.0660</t>
+  </si>
+  <si>
+    <t>0.1234</t>
+  </si>
+  <si>
+    <t>0.9634</t>
+  </si>
+  <si>
+    <t>0.5931</t>
+  </si>
+  <si>
+    <t>0.2703</t>
+  </si>
+  <si>
+    <t>0.0165</t>
+  </si>
+  <si>
+    <t>0.0312</t>
+  </si>
+  <si>
+    <t>0.6255</t>
+  </si>
+  <si>
+    <t>0.5761</t>
+  </si>
+  <si>
+    <t>0.3000</t>
+  </si>
+  <si>
+    <t>0.0146</t>
+  </si>
+  <si>
+    <t>0.0278</t>
+  </si>
+  <si>
+    <t>25.8993</t>
+  </si>
+  <si>
+    <t>6.6173</t>
+  </si>
+  <si>
+    <t>361.6414</t>
+  </si>
+  <si>
+    <t>3.5207</t>
+  </si>
+  <si>
+    <t>0.8171</t>
+  </si>
+  <si>
+    <t>0.6904</t>
+  </si>
+  <si>
+    <t>0.580</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -800,8 +1400,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -823,6 +1430,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1071,7 +1684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1083,20 +1696,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1122,9 +1726,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1154,12 +1755,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1182,9 +1777,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1219,6 +1811,244 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1535,8 +2365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA583CC-99ED-4BBF-8AB4-6DAECB67224B}">
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,35 +2394,35 @@
     <col min="23" max="23" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="145" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="55" t="s">
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
+      <c r="H1" s="144"/>
+      <c r="I1" s="144"/>
+      <c r="J1" s="144"/>
+      <c r="K1" s="144"/>
+      <c r="L1" s="144"/>
+      <c r="M1" s="144"/>
+      <c r="N1" s="144"/>
+      <c r="O1" s="144"/>
+      <c r="P1" s="144"/>
+      <c r="Q1" s="146" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="11"/>
-      <c r="S1" s="59" t="s">
+      <c r="R1" s="147"/>
+      <c r="S1" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="T1" s="74" t="s">
+      <c r="T1" s="67" t="s">
         <v>202</v>
       </c>
       <c r="U1" s="5" t="s">
@@ -1601,175 +2431,175 @@
       <c r="V1" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="W1" s="81" t="s">
+      <c r="W1" s="74" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="145"/>
+      <c r="B2" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
       <c r="F2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="143" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="9" t="s">
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="142"/>
+      <c r="K2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="143" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="8" t="s">
+      <c r="M2" s="142"/>
+      <c r="N2" s="142"/>
+      <c r="O2" s="142"/>
+      <c r="P2" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="Q2" s="56" t="s">
+      <c r="Q2" s="148" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="59" t="s">
+      <c r="R2" s="149"/>
+      <c r="S2" s="53" t="s">
         <v>198</v>
       </c>
-      <c r="T2" s="75"/>
+      <c r="T2" s="68"/>
       <c r="U2" s="5" t="s">
         <v>205</v>
       </c>
       <c r="V2" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="W2" s="21"/>
+      <c r="W2" s="18"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
-      <c r="B3" s="63" t="s">
+      <c r="A3" s="145"/>
+      <c r="B3" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="64" t="s">
+      <c r="E3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="63" t="s">
+      <c r="G3" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="64" t="s">
+      <c r="H3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="64" t="s">
+      <c r="I3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="64" t="s">
+      <c r="J3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="65" t="s">
+      <c r="K3" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="63" t="s">
+      <c r="L3" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="M3" s="64" t="s">
+      <c r="M3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="64" t="s">
+      <c r="N3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="64" t="s">
+      <c r="O3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="66" t="s">
+      <c r="P3" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="Q3" s="63" t="s">
+      <c r="Q3" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="67" t="s">
+      <c r="R3" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="68" t="s">
+      <c r="S3" s="62" t="s">
         <v>197</v>
       </c>
-      <c r="T3" s="63"/>
-      <c r="U3" s="76"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="82"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="69"/>
+      <c r="V3" s="69"/>
+      <c r="W3" s="75"/>
     </row>
     <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="K4" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="N4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="78" t="s">
+      <c r="P4" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="Q4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="19" t="s">
+      <c r="R4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="72" t="s">
+      <c r="S4" s="65" t="s">
         <v>215</v>
       </c>
-      <c r="T4" s="28" t="s">
+      <c r="T4" s="25" t="s">
         <v>216</v>
       </c>
       <c r="U4" s="4" t="s">
@@ -1778,282 +2608,282 @@
       <c r="V4" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="W4" s="14">
+      <c r="W4" s="11">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="78" t="s">
         <v>208</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="15" t="s">
+      <c r="N5" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="P5" s="16" t="s">
+      <c r="P5" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="Q5" s="17" t="s">
+      <c r="Q5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="R5" s="19" t="s">
+      <c r="R5" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="S5" s="72" t="s">
+      <c r="S5" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="T5" s="17" t="s">
+      <c r="T5" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="U5" s="43" t="s">
+      <c r="U5" s="39" t="s">
         <v>205</v>
       </c>
-      <c r="V5" s="43" t="s">
+      <c r="V5" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="W5" s="20">
+      <c r="W5" s="17">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="85" t="s">
+    <row r="6" spans="1:23" s="43" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="78" t="s">
         <v>209</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="39" t="s">
         <v>228</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="39" t="s">
         <v>225</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="39" t="s">
         <v>229</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="40" t="s">
         <v>230</v>
       </c>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="H6" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="J6" s="43" t="s">
+      <c r="J6" s="39" t="s">
         <v>225</v>
       </c>
-      <c r="K6" s="45" t="s">
+      <c r="K6" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="L6" s="42" t="s">
+      <c r="L6" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="M6" s="43" t="s">
+      <c r="M6" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="N6" s="43" t="s">
+      <c r="N6" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="O6" s="43" t="s">
+      <c r="O6" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="P6" s="88" t="s">
+      <c r="P6" s="81" t="s">
         <v>235</v>
       </c>
-      <c r="Q6" s="42" t="s">
+      <c r="Q6" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="R6" s="46" t="s">
+      <c r="R6" s="42" t="s">
         <v>222</v>
       </c>
-      <c r="S6" s="72" t="s">
+      <c r="S6" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="T6" s="17" t="s">
+      <c r="T6" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="U6" s="43" t="s">
+      <c r="U6" s="39" t="s">
         <v>205</v>
       </c>
-      <c r="V6" s="43" t="s">
+      <c r="V6" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="W6" s="41">
+      <c r="W6" s="37">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="85" t="s">
+      <c r="A7" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="52" t="s">
+      <c r="H7" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="K7" s="54" t="s">
+      <c r="K7" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="L7" s="32" t="s">
+      <c r="L7" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="M7" s="32" t="s">
+      <c r="M7" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="N7" s="32" t="s">
+      <c r="N7" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="O7" s="32" t="s">
+      <c r="O7" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="P7" s="50" t="s">
+      <c r="P7" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="Q7" s="34" t="s">
+      <c r="Q7" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="R7" s="35" t="s">
+      <c r="R7" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="S7" s="61" t="s">
+      <c r="S7" s="55" t="s">
         <v>212</v>
       </c>
-      <c r="T7" s="17" t="s">
+      <c r="T7" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="U7" s="43" t="s">
+      <c r="U7" s="39" t="s">
         <v>205</v>
       </c>
-      <c r="V7" s="80" t="s">
+      <c r="V7" s="73" t="s">
         <v>206</v>
       </c>
-      <c r="W7" s="83">
+      <c r="W7" s="76">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="64" t="s">
         <v>210</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="38" t="s">
+      <c r="I8" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="31" t="s">
+      <c r="J8" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="K8" s="53" t="s">
+      <c r="K8" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="L8" s="31" t="s">
+      <c r="L8" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="M8" s="31" t="s">
+      <c r="M8" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="N8" s="31" t="s">
+      <c r="N8" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="O8" s="31" t="s">
+      <c r="O8" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="P8" s="51" t="s">
+      <c r="P8" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="Q8" s="37" t="s">
+      <c r="Q8" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="R8" s="48" t="s">
+      <c r="R8" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="S8" s="73" t="s">
+      <c r="S8" s="66" t="s">
         <v>211</v>
       </c>
-      <c r="T8" s="23" t="s">
+      <c r="T8" s="20" t="s">
         <v>216</v>
       </c>
       <c r="U8" s="3" t="s">
@@ -2062,209 +2892,209 @@
       <c r="V8" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="W8" s="22">
+      <c r="W8" s="19">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="30" t="s">
+      <c r="E9" s="26"/>
+      <c r="F9" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="K9" s="58">
+      <c r="K9" s="52">
         <v>7289</v>
       </c>
-      <c r="L9" s="28" t="s">
+      <c r="L9" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="M9" s="29" t="s">
+      <c r="M9" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="N9" s="29" t="s">
+      <c r="N9" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="O9" s="29" t="s">
+      <c r="O9" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="P9" s="30" t="s">
+      <c r="P9" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="Q9" s="39" t="s">
+      <c r="Q9" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="R9" s="49" t="s">
+      <c r="R9" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="S9" s="60" t="s">
+      <c r="S9" s="54" t="s">
         <v>199</v>
       </c>
-      <c r="T9" s="28" t="s">
+      <c r="T9" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="U9" s="79" t="s">
+      <c r="U9" s="72" t="s">
         <v>205</v>
       </c>
-      <c r="V9" s="79" t="s">
+      <c r="V9" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="W9" s="20">
+      <c r="W9" s="17">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="86" t="s">
+      <c r="A10" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="K10" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="L10" s="17" t="s">
+      <c r="L10" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="N10" s="15" t="s">
+      <c r="N10" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="O10" s="15" t="s">
+      <c r="O10" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="P10" s="16" t="s">
+      <c r="P10" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="Q10" s="17" t="s">
+      <c r="Q10" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="R10" s="19" t="s">
+      <c r="R10" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="S10" s="60" t="s">
+      <c r="S10" s="54" t="s">
         <v>200</v>
       </c>
-      <c r="T10" s="17" t="s">
+      <c r="T10" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="U10" s="43" t="s">
+      <c r="U10" s="39" t="s">
         <v>205</v>
       </c>
-      <c r="V10" s="43" t="s">
+      <c r="V10" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="W10" s="20">
+      <c r="W10" s="17">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="64" t="s">
         <v>213</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="I11" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="J11" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="K11" s="26" t="s">
+      <c r="K11" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="L11" s="23" t="s">
+      <c r="L11" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="M11" s="24" t="s">
+      <c r="M11" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="O11" s="24" t="s">
+      <c r="O11" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="P11" s="25" t="s">
+      <c r="P11" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="Q11" s="23" t="s">
+      <c r="Q11" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="R11" s="27" t="s">
+      <c r="R11" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="S11" s="62" t="s">
+      <c r="S11" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="T11" s="23" t="s">
+      <c r="T11" s="20" t="s">
         <v>216</v>
       </c>
       <c r="U11" s="3" t="s">
@@ -2273,278 +3103,278 @@
       <c r="V11" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="W11" s="22">
+      <c r="W11" s="19">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="84" t="s">
+      <c r="A12" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="J12" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="L12" s="17" t="s">
+      <c r="L12" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="N12" s="15" t="s">
+      <c r="N12" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="O12" s="15" t="s">
+      <c r="O12" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="P12" s="78" t="s">
+      <c r="P12" s="71" t="s">
         <v>149</v>
       </c>
-      <c r="Q12" s="17" t="s">
+      <c r="Q12" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="R12" s="19" t="s">
+      <c r="R12" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="S12" s="20" t="s">
+      <c r="S12" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="T12" s="17" t="s">
+      <c r="T12" s="14" t="s">
         <v>217</v>
       </c>
       <c r="U12" s="2"/>
-      <c r="V12" s="77" t="s">
+      <c r="V12" s="70" t="s">
         <v>206</v>
       </c>
-      <c r="W12" s="20">
+      <c r="W12" s="17">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="87" t="s">
+      <c r="A13" s="80" t="s">
         <v>150</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="K13" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="L13" s="17" t="s">
+      <c r="L13" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="M13" s="15" t="s">
+      <c r="M13" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="N13" s="15" t="s">
+      <c r="N13" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="O13" s="15" t="s">
+      <c r="O13" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="P13" s="78" t="s">
+      <c r="P13" s="71" t="s">
         <v>166</v>
       </c>
-      <c r="Q13" s="17" t="s">
+      <c r="Q13" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="R13" s="19" t="s">
+      <c r="R13" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="S13" s="20" t="s">
+      <c r="S13" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="T13" s="17" t="s">
+      <c r="T13" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="U13" s="43" t="s">
+      <c r="U13" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="V13" s="43" t="s">
+      <c r="V13" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="W13" s="20">
+      <c r="W13" s="17">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="86" t="s">
+      <c r="A14" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="I14" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="J14" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="K14" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="L14" s="17" t="s">
+      <c r="L14" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="M14" s="15" t="s">
+      <c r="M14" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="N14" s="15" t="s">
+      <c r="N14" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="O14" s="15" t="s">
+      <c r="O14" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="P14" s="16" t="s">
+      <c r="P14" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="Q14" s="16" t="s">
+      <c r="Q14" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="R14" s="19" t="s">
+      <c r="R14" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="S14" s="20" t="s">
+      <c r="S14" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="T14" s="17" t="s">
+      <c r="T14" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="U14" s="43" t="s">
+      <c r="U14" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="V14" s="43" t="s">
+      <c r="V14" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="W14" s="20">
+      <c r="W14" s="17">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="J15" s="24" t="s">
+      <c r="J15" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="K15" s="26" t="s">
+      <c r="K15" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="L15" s="23" t="s">
+      <c r="L15" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="M15" s="24" t="s">
+      <c r="M15" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="N15" s="24" t="s">
+      <c r="N15" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="O15" s="24" t="s">
+      <c r="O15" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="23" t="s">
+      <c r="P15" s="22"/>
+      <c r="Q15" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="R15" s="27" t="s">
+      <c r="R15" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="S15" s="22" t="s">
+      <c r="S15" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="T15" s="23" t="s">
+      <c r="T15" s="20" t="s">
         <v>217</v>
       </c>
       <c r="U15" s="3" t="s">
@@ -2553,7 +3383,7 @@
       <c r="V15" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="W15" s="22">
+      <c r="W15" s="19">
         <v>23</v>
       </c>
     </row>
@@ -2570,4 +3400,1202 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A0290E-A5D1-4EAC-B47A-7E70F99F3CE5}">
+  <dimension ref="A1:S15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="5.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="150" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="151" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="152"/>
+      <c r="H1" s="152"/>
+      <c r="I1" s="152"/>
+      <c r="J1" s="152"/>
+      <c r="K1" s="152"/>
+      <c r="L1" s="152"/>
+      <c r="M1" s="152"/>
+      <c r="N1" s="152"/>
+      <c r="O1" s="152"/>
+      <c r="P1" s="153"/>
+      <c r="Q1" s="85" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="150"/>
+      <c r="B2" s="143" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="143" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="142"/>
+      <c r="K2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="143" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="142"/>
+      <c r="N2" s="142"/>
+      <c r="O2" s="142"/>
+      <c r="P2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q2" s="51" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="150"/>
+      <c r="B3" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="84" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="82" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="84" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="82" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="84" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="82" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="75"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="77" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="90" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" s="91" t="s">
+        <v>280</v>
+      </c>
+      <c r="D4" s="91" t="s">
+        <v>281</v>
+      </c>
+      <c r="E4" s="91" t="s">
+        <v>282</v>
+      </c>
+      <c r="F4" s="92" t="s">
+        <v>283</v>
+      </c>
+      <c r="G4" s="90" t="s">
+        <v>284</v>
+      </c>
+      <c r="H4" s="91" t="s">
+        <v>285</v>
+      </c>
+      <c r="I4" s="91" t="s">
+        <v>261</v>
+      </c>
+      <c r="J4" s="91" t="s">
+        <v>286</v>
+      </c>
+      <c r="K4" s="93" t="s">
+        <v>287</v>
+      </c>
+      <c r="L4" s="90" t="s">
+        <v>288</v>
+      </c>
+      <c r="M4" s="91" t="s">
+        <v>289</v>
+      </c>
+      <c r="N4" s="91" t="s">
+        <v>290</v>
+      </c>
+      <c r="O4" s="91" t="s">
+        <v>291</v>
+      </c>
+      <c r="P4" s="94" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="86">
+        <v>12</v>
+      </c>
+      <c r="R4" s="43"/>
+    </row>
+    <row r="5" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="78" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5" s="90" t="s">
+        <v>428</v>
+      </c>
+      <c r="C5" s="91" t="s">
+        <v>296</v>
+      </c>
+      <c r="D5" s="91" t="s">
+        <v>297</v>
+      </c>
+      <c r="E5" s="91" t="s">
+        <v>298</v>
+      </c>
+      <c r="F5" s="92" t="s">
+        <v>299</v>
+      </c>
+      <c r="G5" s="90" t="s">
+        <v>300</v>
+      </c>
+      <c r="H5" s="91" t="s">
+        <v>301</v>
+      </c>
+      <c r="I5" s="91" t="s">
+        <v>263</v>
+      </c>
+      <c r="J5" s="91" t="s">
+        <v>302</v>
+      </c>
+      <c r="K5" s="92" t="s">
+        <v>303</v>
+      </c>
+      <c r="L5" s="90" t="s">
+        <v>304</v>
+      </c>
+      <c r="M5" s="91" t="s">
+        <v>305</v>
+      </c>
+      <c r="N5" s="91" t="s">
+        <v>306</v>
+      </c>
+      <c r="O5" s="91" t="s">
+        <v>307</v>
+      </c>
+      <c r="P5" s="92" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>13</v>
+      </c>
+      <c r="R5" s="43"/>
+    </row>
+    <row r="6" spans="1:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="78" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" s="95" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" s="96" t="s">
+        <v>269</v>
+      </c>
+      <c r="D6" s="96" t="s">
+        <v>270</v>
+      </c>
+      <c r="E6" s="96" t="s">
+        <v>271</v>
+      </c>
+      <c r="F6" s="97" t="s">
+        <v>272</v>
+      </c>
+      <c r="G6" s="95" t="s">
+        <v>273</v>
+      </c>
+      <c r="H6" s="96" t="s">
+        <v>274</v>
+      </c>
+      <c r="I6" s="96" t="s">
+        <v>275</v>
+      </c>
+      <c r="J6" s="96" t="s">
+        <v>258</v>
+      </c>
+      <c r="K6" s="98" t="s">
+        <v>259</v>
+      </c>
+      <c r="L6" s="95" t="s">
+        <v>276</v>
+      </c>
+      <c r="M6" s="96" t="s">
+        <v>277</v>
+      </c>
+      <c r="N6" s="96" t="s">
+        <v>84</v>
+      </c>
+      <c r="O6" s="96" t="s">
+        <v>278</v>
+      </c>
+      <c r="P6" s="161" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="87">
+        <v>14</v>
+      </c>
+      <c r="R6" s="43"/>
+      <c r="S6" s="162"/>
+    </row>
+    <row r="7" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="78" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="99" t="s">
+        <v>310</v>
+      </c>
+      <c r="C7" s="93" t="s">
+        <v>311</v>
+      </c>
+      <c r="D7" s="93" t="s">
+        <v>312</v>
+      </c>
+      <c r="E7" s="93" t="s">
+        <v>313</v>
+      </c>
+      <c r="F7" s="92" t="s">
+        <v>314</v>
+      </c>
+      <c r="G7" s="99" t="s">
+        <v>315</v>
+      </c>
+      <c r="H7" s="89" t="s">
+        <v>316</v>
+      </c>
+      <c r="I7" s="93" t="s">
+        <v>260</v>
+      </c>
+      <c r="J7" s="93" t="s">
+        <v>233</v>
+      </c>
+      <c r="K7" s="100" t="s">
+        <v>317</v>
+      </c>
+      <c r="L7" s="93" t="s">
+        <v>318</v>
+      </c>
+      <c r="M7" s="93" t="s">
+        <v>305</v>
+      </c>
+      <c r="N7" s="93" t="s">
+        <v>266</v>
+      </c>
+      <c r="O7" s="93" t="s">
+        <v>319</v>
+      </c>
+      <c r="P7" s="101" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>15</v>
+      </c>
+      <c r="R7" s="43"/>
+    </row>
+    <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="64" t="s">
+        <v>210</v>
+      </c>
+      <c r="B8" s="99" t="s">
+        <v>322</v>
+      </c>
+      <c r="C8" s="93" t="s">
+        <v>323</v>
+      </c>
+      <c r="D8" s="93" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="93" t="s">
+        <v>324</v>
+      </c>
+      <c r="F8" s="92" t="s">
+        <v>325</v>
+      </c>
+      <c r="G8" s="102" t="s">
+        <v>326</v>
+      </c>
+      <c r="H8" s="103" t="s">
+        <v>327</v>
+      </c>
+      <c r="I8" s="103" t="s">
+        <v>328</v>
+      </c>
+      <c r="J8" s="93" t="s">
+        <v>329</v>
+      </c>
+      <c r="K8" s="104" t="s">
+        <v>330</v>
+      </c>
+      <c r="L8" s="123" t="s">
+        <v>331</v>
+      </c>
+      <c r="M8" s="93" t="s">
+        <v>153</v>
+      </c>
+      <c r="N8" s="93" t="s">
+        <v>332</v>
+      </c>
+      <c r="O8" s="93" t="s">
+        <v>333</v>
+      </c>
+      <c r="P8" s="105" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q8" s="88">
+        <v>16</v>
+      </c>
+      <c r="R8" s="43"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="106" t="s">
+        <v>336</v>
+      </c>
+      <c r="C9" s="107" t="s">
+        <v>337</v>
+      </c>
+      <c r="D9" s="107" t="s">
+        <v>338</v>
+      </c>
+      <c r="E9" s="107" t="s">
+        <v>339</v>
+      </c>
+      <c r="F9" s="108" t="s">
+        <v>340</v>
+      </c>
+      <c r="G9" s="109" t="s">
+        <v>341</v>
+      </c>
+      <c r="H9" s="110" t="s">
+        <v>342</v>
+      </c>
+      <c r="I9" s="110" t="s">
+        <v>343</v>
+      </c>
+      <c r="J9" s="107" t="s">
+        <v>344</v>
+      </c>
+      <c r="K9" s="108" t="s">
+        <v>345</v>
+      </c>
+      <c r="L9" s="106" t="s">
+        <v>346</v>
+      </c>
+      <c r="M9" s="107" t="s">
+        <v>347</v>
+      </c>
+      <c r="N9" s="107" t="s">
+        <v>348</v>
+      </c>
+      <c r="O9" s="107" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="108" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>17</v>
+      </c>
+      <c r="R9" s="43"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="79" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="90" t="s">
+        <v>351</v>
+      </c>
+      <c r="C10" s="91" t="s">
+        <v>352</v>
+      </c>
+      <c r="D10" s="91" t="s">
+        <v>353</v>
+      </c>
+      <c r="E10" s="91" t="s">
+        <v>354</v>
+      </c>
+      <c r="F10" s="111" t="s">
+        <v>355</v>
+      </c>
+      <c r="G10" s="90" t="s">
+        <v>356</v>
+      </c>
+      <c r="H10" s="91" t="s">
+        <v>350</v>
+      </c>
+      <c r="I10" s="91" t="s">
+        <v>107</v>
+      </c>
+      <c r="J10" s="91" t="s">
+        <v>357</v>
+      </c>
+      <c r="K10" s="92" t="s">
+        <v>358</v>
+      </c>
+      <c r="L10" s="90" t="s">
+        <v>359</v>
+      </c>
+      <c r="M10" s="91" t="s">
+        <v>360</v>
+      </c>
+      <c r="N10" s="91" t="s">
+        <v>144</v>
+      </c>
+      <c r="O10" s="91" t="s">
+        <v>361</v>
+      </c>
+      <c r="P10" s="92" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q10" s="9">
+        <v>18</v>
+      </c>
+      <c r="R10" s="43"/>
+    </row>
+    <row r="11" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="64" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" s="112" t="s">
+        <v>364</v>
+      </c>
+      <c r="C11" s="113" t="s">
+        <v>365</v>
+      </c>
+      <c r="D11" s="113" t="s">
+        <v>366</v>
+      </c>
+      <c r="E11" s="113" t="s">
+        <v>367</v>
+      </c>
+      <c r="F11" s="114" t="s">
+        <v>368</v>
+      </c>
+      <c r="G11" s="112" t="s">
+        <v>369</v>
+      </c>
+      <c r="H11" s="113" t="s">
+        <v>370</v>
+      </c>
+      <c r="I11" s="113" t="s">
+        <v>188</v>
+      </c>
+      <c r="J11" s="113" t="s">
+        <v>371</v>
+      </c>
+      <c r="K11" s="115" t="s">
+        <v>372</v>
+      </c>
+      <c r="L11" s="163" t="s">
+        <v>373</v>
+      </c>
+      <c r="M11" s="113" t="s">
+        <v>374</v>
+      </c>
+      <c r="N11" s="113" t="s">
+        <v>375</v>
+      </c>
+      <c r="O11" s="113" t="s">
+        <v>376</v>
+      </c>
+      <c r="P11" s="115" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q11" s="88">
+        <v>19</v>
+      </c>
+      <c r="R11" s="43"/>
+    </row>
+    <row r="12" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="137" t="s">
+        <v>251</v>
+      </c>
+      <c r="B12" s="90" t="s">
+        <v>379</v>
+      </c>
+      <c r="C12" s="91" t="s">
+        <v>380</v>
+      </c>
+      <c r="D12" s="91" t="s">
+        <v>268</v>
+      </c>
+      <c r="E12" s="91" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="111" t="s">
+        <v>381</v>
+      </c>
+      <c r="G12" s="90" t="s">
+        <v>382</v>
+      </c>
+      <c r="H12" s="91" t="s">
+        <v>383</v>
+      </c>
+      <c r="I12" s="91" t="s">
+        <v>155</v>
+      </c>
+      <c r="J12" s="91">
+        <v>357</v>
+      </c>
+      <c r="K12" s="92" t="s">
+        <v>384</v>
+      </c>
+      <c r="L12" s="95" t="s">
+        <v>385</v>
+      </c>
+      <c r="M12" s="91" t="s">
+        <v>153</v>
+      </c>
+      <c r="N12" s="91" t="s">
+        <v>386</v>
+      </c>
+      <c r="O12" s="91" t="s">
+        <v>387</v>
+      </c>
+      <c r="P12" s="94" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>20</v>
+      </c>
+      <c r="R12" s="43"/>
+      <c r="S12" s="162"/>
+    </row>
+    <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="138" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" s="90" t="s">
+        <v>390</v>
+      </c>
+      <c r="C13" s="91">
+        <v>9384</v>
+      </c>
+      <c r="D13" s="91" t="s">
+        <v>175</v>
+      </c>
+      <c r="E13" s="91" t="s">
+        <v>391</v>
+      </c>
+      <c r="F13" s="111" t="s">
+        <v>392</v>
+      </c>
+      <c r="G13" s="90" t="s">
+        <v>393</v>
+      </c>
+      <c r="H13" s="91" t="s">
+        <v>394</v>
+      </c>
+      <c r="I13" s="91" t="s">
+        <v>144</v>
+      </c>
+      <c r="J13" s="91" t="s">
+        <v>264</v>
+      </c>
+      <c r="K13" s="92">
+        <v>7199</v>
+      </c>
+      <c r="L13" s="95" t="s">
+        <v>265</v>
+      </c>
+      <c r="M13" s="91" t="s">
+        <v>262</v>
+      </c>
+      <c r="N13" s="91" t="s">
+        <v>266</v>
+      </c>
+      <c r="O13" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="P13" s="94" t="s">
+        <v>341</v>
+      </c>
+      <c r="Q13" s="9">
+        <v>21</v>
+      </c>
+      <c r="R13" s="43"/>
+      <c r="S13" s="162"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="90" t="s">
+        <v>410</v>
+      </c>
+      <c r="C14" s="91" t="s">
+        <v>411</v>
+      </c>
+      <c r="D14" s="91" t="s">
+        <v>412</v>
+      </c>
+      <c r="E14" s="91" t="s">
+        <v>413</v>
+      </c>
+      <c r="F14" s="111" t="s">
+        <v>414</v>
+      </c>
+      <c r="G14" s="90" t="s">
+        <v>415</v>
+      </c>
+      <c r="H14" s="91" t="s">
+        <v>416</v>
+      </c>
+      <c r="I14" s="91" t="s">
+        <v>417</v>
+      </c>
+      <c r="J14" s="91" t="s">
+        <v>418</v>
+      </c>
+      <c r="K14" s="92" t="s">
+        <v>419</v>
+      </c>
+      <c r="L14" s="90" t="s">
+        <v>420</v>
+      </c>
+      <c r="M14" s="91" t="s">
+        <v>421</v>
+      </c>
+      <c r="N14" s="91" t="s">
+        <v>422</v>
+      </c>
+      <c r="O14" s="91" t="s">
+        <v>423</v>
+      </c>
+      <c r="P14" s="92" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q14" s="9">
+        <v>22</v>
+      </c>
+      <c r="R14" s="43"/>
+    </row>
+    <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="64" t="s">
+        <v>252</v>
+      </c>
+      <c r="B15" s="112" t="s">
+        <v>395</v>
+      </c>
+      <c r="C15" s="113" t="s">
+        <v>396</v>
+      </c>
+      <c r="D15" s="113" t="s">
+        <v>397</v>
+      </c>
+      <c r="E15" s="113" t="s">
+        <v>398</v>
+      </c>
+      <c r="F15" s="114" t="s">
+        <v>399</v>
+      </c>
+      <c r="G15" s="112" t="s">
+        <v>400</v>
+      </c>
+      <c r="H15" s="113" t="s">
+        <v>401</v>
+      </c>
+      <c r="I15" s="113" t="s">
+        <v>397</v>
+      </c>
+      <c r="J15" s="113" t="s">
+        <v>402</v>
+      </c>
+      <c r="K15" s="115" t="s">
+        <v>403</v>
+      </c>
+      <c r="L15" s="112" t="s">
+        <v>404</v>
+      </c>
+      <c r="M15" s="113" t="s">
+        <v>405</v>
+      </c>
+      <c r="N15" s="113" t="s">
+        <v>406</v>
+      </c>
+      <c r="O15" s="113" t="s">
+        <v>407</v>
+      </c>
+      <c r="P15" s="115" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q15" s="88">
+        <v>23</v>
+      </c>
+      <c r="R15" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="L2:O2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31830DC9-08FB-4050-8B0D-C5E24AEC0034}">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18" style="43" customWidth="1"/>
+    <col min="10" max="16" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="145" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="146" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="147"/>
+      <c r="D1" s="53" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1" s="154" t="s">
+        <v>238</v>
+      </c>
+      <c r="F1" s="157" t="s">
+        <v>241</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="H1" s="117" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="145"/>
+      <c r="B2" s="148" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="149"/>
+      <c r="D2" s="53" t="s">
+        <v>240</v>
+      </c>
+      <c r="E2" s="155"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="H2" s="118"/>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="145"/>
+      <c r="B3" s="83" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="116" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="62" t="s">
+        <v>242</v>
+      </c>
+      <c r="E3" s="156"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="120"/>
+    </row>
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="77" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="90" t="s">
+        <v>292</v>
+      </c>
+      <c r="C4" s="126" t="s">
+        <v>293</v>
+      </c>
+      <c r="D4" s="127" t="s">
+        <v>243</v>
+      </c>
+      <c r="E4" s="106" t="s">
+        <v>216</v>
+      </c>
+      <c r="F4" s="121" t="s">
+        <v>205</v>
+      </c>
+      <c r="G4" s="121" t="s">
+        <v>206</v>
+      </c>
+      <c r="H4" s="86">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="78" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5" s="90" t="s">
+        <v>308</v>
+      </c>
+      <c r="C5" s="126" t="s">
+        <v>309</v>
+      </c>
+      <c r="D5" s="127" t="s">
+        <v>244</v>
+      </c>
+      <c r="E5" s="90" t="s">
+        <v>216</v>
+      </c>
+      <c r="F5" s="96" t="s">
+        <v>205</v>
+      </c>
+      <c r="G5" s="96" t="s">
+        <v>206</v>
+      </c>
+      <c r="H5" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="78" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" s="95" t="s">
+        <v>294</v>
+      </c>
+      <c r="C6" s="128" t="s">
+        <v>295</v>
+      </c>
+      <c r="D6" s="127" t="s">
+        <v>244</v>
+      </c>
+      <c r="E6" s="90" t="s">
+        <v>216</v>
+      </c>
+      <c r="F6" s="96" t="s">
+        <v>205</v>
+      </c>
+      <c r="G6" s="96" t="s">
+        <v>206</v>
+      </c>
+      <c r="H6" s="87">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="78" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="99" t="s">
+        <v>320</v>
+      </c>
+      <c r="C7" s="129" t="s">
+        <v>321</v>
+      </c>
+      <c r="D7" s="130" t="s">
+        <v>245</v>
+      </c>
+      <c r="E7" s="90" t="s">
+        <v>216</v>
+      </c>
+      <c r="F7" s="96" t="s">
+        <v>205</v>
+      </c>
+      <c r="G7" s="96" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="64" t="s">
+        <v>210</v>
+      </c>
+      <c r="B8" s="102" t="s">
+        <v>334</v>
+      </c>
+      <c r="C8" s="131" t="s">
+        <v>335</v>
+      </c>
+      <c r="D8" s="132" t="s">
+        <v>244</v>
+      </c>
+      <c r="E8" s="112" t="s">
+        <v>216</v>
+      </c>
+      <c r="F8" s="122" t="s">
+        <v>205</v>
+      </c>
+      <c r="G8" s="122" t="s">
+        <v>206</v>
+      </c>
+      <c r="H8" s="88">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="109" t="s">
+        <v>349</v>
+      </c>
+      <c r="C9" s="133" t="s">
+        <v>350</v>
+      </c>
+      <c r="D9" s="134" t="s">
+        <v>247</v>
+      </c>
+      <c r="E9" s="106" t="s">
+        <v>216</v>
+      </c>
+      <c r="F9" s="123" t="s">
+        <v>205</v>
+      </c>
+      <c r="G9" s="123" t="s">
+        <v>206</v>
+      </c>
+      <c r="H9" s="9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="79" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="90" t="s">
+        <v>362</v>
+      </c>
+      <c r="C10" s="126" t="s">
+        <v>363</v>
+      </c>
+      <c r="D10" s="134" t="s">
+        <v>246</v>
+      </c>
+      <c r="E10" s="90" t="s">
+        <v>216</v>
+      </c>
+      <c r="F10" s="96" t="s">
+        <v>205</v>
+      </c>
+      <c r="G10" s="96" t="s">
+        <v>206</v>
+      </c>
+      <c r="H10" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="64" t="s">
+        <v>213</v>
+      </c>
+      <c r="B11" s="112" t="s">
+        <v>377</v>
+      </c>
+      <c r="C11" s="135" t="s">
+        <v>378</v>
+      </c>
+      <c r="D11" s="136" t="s">
+        <v>248</v>
+      </c>
+      <c r="E11" s="112" t="s">
+        <v>216</v>
+      </c>
+      <c r="F11" s="122" t="s">
+        <v>205</v>
+      </c>
+      <c r="G11" s="122" t="s">
+        <v>206</v>
+      </c>
+      <c r="H11" s="88">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="137" t="s">
+        <v>253</v>
+      </c>
+      <c r="B12" s="90" t="s">
+        <v>388</v>
+      </c>
+      <c r="C12" s="126" t="s">
+        <v>389</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E12" s="139" t="s">
+        <v>256</v>
+      </c>
+      <c r="F12" s="124"/>
+      <c r="G12" s="125" t="s">
+        <v>206</v>
+      </c>
+      <c r="H12" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="80" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="90" t="s">
+        <v>426</v>
+      </c>
+      <c r="C13" s="126" t="s">
+        <v>427</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E13" s="90" t="s">
+        <v>218</v>
+      </c>
+      <c r="F13" s="96" t="s">
+        <v>204</v>
+      </c>
+      <c r="G13" s="96" t="s">
+        <v>206</v>
+      </c>
+      <c r="H13" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="111" t="s">
+        <v>424</v>
+      </c>
+      <c r="C14" s="126" t="s">
+        <v>425</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E14" s="90" t="s">
+        <v>216</v>
+      </c>
+      <c r="F14" s="96" t="s">
+        <v>204</v>
+      </c>
+      <c r="G14" s="96" t="s">
+        <v>206</v>
+      </c>
+      <c r="H14" s="9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="64" t="s">
+        <v>252</v>
+      </c>
+      <c r="B15" s="112" t="s">
+        <v>408</v>
+      </c>
+      <c r="C15" s="160" t="s">
+        <v>409</v>
+      </c>
+      <c r="D15" s="88" t="s">
+        <v>249</v>
+      </c>
+      <c r="E15" s="140" t="s">
+        <v>257</v>
+      </c>
+      <c r="F15" s="122" t="s">
+        <v>205</v>
+      </c>
+      <c r="G15" s="122" t="s">
+        <v>207</v>
+      </c>
+      <c r="H15" s="88">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>